<commit_message>
Data augmentation added (todo: change model)
</commit_message>
<xml_diff>
--- a/dataset/Mapper.xlsx
+++ b/dataset/Mapper.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1513,6 +1513,282 @@
         </is>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>image89.jpg</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Andromeda</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>image90.jpg</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Andromeda</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>image91.jpg</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Andromeda</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>image92.jpg</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Andromeda</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>image93.jpg</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Antlia</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>image94.jpg</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Antlia</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>image95.jpg</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Antlia</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>image96.jpg</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Antlia</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>image97.jpg</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Antlia</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>image98.jpg</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Apus</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>image99.jpg</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Apus</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>image100.jpg</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Apus</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>image101.jpg</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Apus</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>image102.jpg</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Apus</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>image103.jpg</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Apus</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>image104.jpg</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Aquarius</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>image105.jpg</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Aquarius</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>image106.jpg</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Aquarius</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>image107.jpg</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Aquarius</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>image108.jpg</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Aquarius</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>image109.jpg</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Aquila</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>image110.jpg</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Aquila</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>image111.jpg</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Aquila</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>